<commit_message>
Backlog on 2 sprint
My tasks for 2 sprint
</commit_message>
<xml_diff>
--- a/Doc/backlog-template.xlsx
+++ b/Doc/backlog-template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\Documents\GitHub\Ask_service\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +36,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="141">
   <si>
     <t>Kokhanov, Yeremenko, Tkachov, Daubur, Danilenko, Kiparenko, Golubchikov</t>
   </si>
@@ -1107,6 +1102,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1119,24 +1132,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1643,6 +1638,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1901,7 +2040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1912,74 +2051,74 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.88671875"/>
-    <col min="2" max="2" width="6.33203125"/>
-    <col min="3" max="3" width="9.33203125"/>
-    <col min="4" max="4" width="11.109375"/>
-    <col min="5" max="5" width="13.6640625"/>
-    <col min="6" max="6" width="42.6640625"/>
-    <col min="7" max="7" width="51.33203125"/>
-    <col min="8" max="8" width="15.6640625"/>
-    <col min="9" max="9" width="25.88671875"/>
+    <col min="1" max="1" width="1.85546875"/>
+    <col min="2" max="2" width="6.28515625"/>
+    <col min="3" max="3" width="9.28515625"/>
+    <col min="4" max="4" width="11.140625"/>
+    <col min="5" max="5" width="13.7109375"/>
+    <col min="6" max="6" width="42.7109375"/>
+    <col min="7" max="7" width="51.28515625"/>
+    <col min="8" max="8" width="15.7109375"/>
+    <col min="9" max="9" width="25.85546875"/>
     <col min="10" max="10" width="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1992,7 +2131,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2158,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
@@ -2027,17 +2166,17 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="15">
         <v>10</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="17">
         <v>1</v>
@@ -2060,7 +2199,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="17">
         <v>2</v>
@@ -2083,7 +2222,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="17">
         <v>3</v>
@@ -2104,7 +2243,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
@@ -2112,10 +2251,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="57"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="23">
         <v>20</v>
       </c>
@@ -2123,7 +2262,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="17">
         <v>4</v>
@@ -2144,7 +2283,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="17">
         <v>5</v>
@@ -2165,7 +2304,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="17">
         <v>6</v>
@@ -2186,7 +2325,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="17">
         <v>7</v>
@@ -2207,7 +2346,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
@@ -2215,10 +2354,10 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="57"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="23">
         <v>4</v>
       </c>
@@ -2226,7 +2365,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="17">
         <v>8</v>
@@ -2249,7 +2388,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="17">
         <v>9</v>
@@ -2272,7 +2411,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
@@ -2280,10 +2419,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="57"/>
+      <c r="G18" s="56"/>
       <c r="H18" s="23">
         <v>8</v>
       </c>
@@ -2291,7 +2430,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="17">
         <v>10</v>
@@ -2314,7 +2453,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="17">
         <v>11</v>
@@ -2337,7 +2476,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
@@ -2345,10 +2484,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="57"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="23">
         <v>8</v>
       </c>
@@ -2356,7 +2495,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <v>12</v>
       </c>
@@ -2376,7 +2515,7 @@
       </c>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <v>13</v>
       </c>
@@ -2396,23 +2535,23 @@
       </c>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="58" t="s">
+      <c r="F24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="58"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="23">
         <v>8</v>
       </c>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <v>14</v>
       </c>
@@ -2430,7 +2569,7 @@
       </c>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>15</v>
       </c>
@@ -2448,23 +2587,23 @@
       </c>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="58" t="s">
+      <c r="F27" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="58"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="23">
         <v>13</v>
       </c>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17">
         <v>16</v>
       </c>
@@ -2482,7 +2621,7 @@
       </c>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <v>17</v>
       </c>
@@ -2500,23 +2639,23 @@
       </c>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="58" t="s">
+      <c r="F30" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="58"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="23">
         <v>12</v>
       </c>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17">
         <v>18</v>
       </c>
@@ -2534,7 +2673,7 @@
       </c>
       <c r="I31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17">
         <v>19</v>
       </c>
@@ -2552,7 +2691,7 @@
       </c>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" spans="2:9" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17">
         <v>20</v>
       </c>
@@ -2570,7 +2709,7 @@
       </c>
       <c r="I33" s="33"/>
     </row>
-    <row r="34" spans="2:9" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
         <v>21</v>
       </c>
@@ -2588,23 +2727,23 @@
       </c>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="58" t="s">
+      <c r="F35" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="58"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="23">
         <v>11</v>
       </c>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" spans="2:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17">
         <v>22</v>
       </c>
@@ -2624,7 +2763,7 @@
       </c>
       <c r="I36" s="33"/>
     </row>
-    <row r="37" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
         <v>23</v>
       </c>
@@ -2642,23 +2781,23 @@
       </c>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
       <c r="C38" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="58" t="s">
+      <c r="F38" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="58"/>
+      <c r="G38" s="54"/>
       <c r="H38" s="23">
         <v>18</v>
       </c>
       <c r="I38" s="33"/>
     </row>
-    <row r="39" spans="2:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
         <v>24</v>
       </c>
@@ -2676,12 +2815,14 @@
       </c>
       <c r="I39" s="33"/>
     </row>
-    <row r="40" spans="2:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="17">
         <v>25</v>
       </c>
       <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
+      <c r="D40" s="29" t="s">
+        <v>14</v>
+      </c>
       <c r="E40" s="30"/>
       <c r="F40" s="31" t="s">
         <v>75</v>
@@ -2694,12 +2835,14 @@
       </c>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="17">
         <v>26</v>
       </c>
       <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
+      <c r="D41" s="29" t="s">
+        <v>14</v>
+      </c>
       <c r="E41" s="30"/>
       <c r="F41" s="34" t="s">
         <v>77</v>
@@ -2712,7 +2855,7 @@
       </c>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" spans="2:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="17">
         <v>27</v>
       </c>
@@ -2730,23 +2873,23 @@
       </c>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
       <c r="C43" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="59" t="s">
+      <c r="F43" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="G43" s="59"/>
+      <c r="G43" s="51"/>
       <c r="H43" s="23">
         <v>11</v>
       </c>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="17">
         <v>28</v>
       </c>
@@ -2764,7 +2907,7 @@
       </c>
       <c r="I44" s="33"/>
     </row>
-    <row r="45" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="17">
         <v>29</v>
       </c>
@@ -2782,7 +2925,7 @@
       </c>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17">
         <v>30</v>
       </c>
@@ -2802,23 +2945,23 @@
       </c>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="37"/>
-      <c r="F47" s="60" t="s">
+      <c r="F47" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="60"/>
+      <c r="G47" s="53"/>
       <c r="H47" s="39">
         <v>6</v>
       </c>
       <c r="I47" s="33"/>
     </row>
-    <row r="48" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="17">
         <v>31</v>
       </c>
@@ -2838,7 +2981,7 @@
       </c>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="17">
         <v>32</v>
       </c>
@@ -2858,7 +3001,7 @@
       </c>
       <c r="I49" s="33"/>
     </row>
-    <row r="50" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="40">
         <v>33</v>
       </c>
@@ -2878,23 +3021,23 @@
       </c>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="40"/>
       <c r="C51" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="37"/>
-      <c r="F51" s="59" t="s">
+      <c r="F51" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="59"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="39">
         <v>5</v>
       </c>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="40">
         <v>34</v>
       </c>
@@ -2912,23 +3055,23 @@
       </c>
       <c r="I52" s="33"/>
     </row>
-    <row r="53" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="40"/>
       <c r="C53" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D53" s="36"/>
       <c r="E53" s="37"/>
-      <c r="F53" s="59" t="s">
+      <c r="F53" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="G53" s="59"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="39">
         <v>7</v>
       </c>
       <c r="I53" s="33"/>
     </row>
-    <row r="54" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="40">
         <v>35</v>
       </c>
@@ -2946,7 +3089,7 @@
       </c>
       <c r="I54" s="33"/>
     </row>
-    <row r="55" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="40">
         <v>36</v>
       </c>
@@ -2964,23 +3107,23 @@
       </c>
       <c r="I55" s="33"/>
     </row>
-    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="40"/>
       <c r="C56" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="37"/>
-      <c r="F56" s="59" t="s">
+      <c r="F56" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="59"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="39">
         <v>10</v>
       </c>
       <c r="I56" s="33"/>
     </row>
-    <row r="57" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="40">
         <v>37</v>
       </c>
@@ -2998,7 +3141,7 @@
       </c>
       <c r="I57" s="33"/>
     </row>
-    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="40">
         <v>38</v>
       </c>
@@ -3016,23 +3159,23 @@
       </c>
       <c r="I58" s="33"/>
     </row>
-    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="40"/>
       <c r="C59" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="37"/>
-      <c r="F59" s="61" t="s">
+      <c r="F59" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="61"/>
+      <c r="G59" s="52"/>
       <c r="H59" s="39">
         <v>4</v>
       </c>
       <c r="I59" s="33"/>
     </row>
-    <row r="60" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="40">
         <v>39</v>
       </c>
@@ -3052,7 +3195,7 @@
       </c>
       <c r="I60" s="33"/>
     </row>
-    <row r="61" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="40">
         <v>40</v>
       </c>
@@ -3072,23 +3215,23 @@
       </c>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="40"/>
       <c r="C62" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="37"/>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="59"/>
+      <c r="G62" s="51"/>
       <c r="H62" s="39">
         <v>5</v>
       </c>
       <c r="I62" s="33"/>
     </row>
-    <row r="63" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="40">
         <v>41</v>
       </c>
@@ -3106,23 +3249,23 @@
       </c>
       <c r="I63" s="33"/>
     </row>
-    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="40"/>
       <c r="C64" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="37"/>
-      <c r="F64" s="59" t="s">
+      <c r="F64" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="G64" s="59"/>
+      <c r="G64" s="51"/>
       <c r="H64" s="39">
         <v>8</v>
       </c>
       <c r="I64" s="33"/>
     </row>
-    <row r="65" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="40">
         <v>42</v>
       </c>
@@ -3140,7 +3283,7 @@
       </c>
       <c r="I65" s="33"/>
     </row>
-    <row r="66" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="40">
         <v>43</v>
       </c>
@@ -3158,7 +3301,7 @@
       </c>
       <c r="I66" s="33"/>
     </row>
-    <row r="67" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="40">
         <v>44</v>
       </c>
@@ -3176,23 +3319,23 @@
       </c>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="40"/>
       <c r="C68" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="37"/>
-      <c r="F68" s="59" t="s">
+      <c r="F68" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="G68" s="59"/>
+      <c r="G68" s="51"/>
       <c r="H68" s="39">
         <v>3</v>
       </c>
       <c r="I68" s="33"/>
     </row>
-    <row r="69" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="40">
         <v>45</v>
       </c>
@@ -3210,23 +3353,23 @@
       </c>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="40"/>
       <c r="C70" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="37"/>
-      <c r="F70" s="59" t="s">
+      <c r="F70" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="59"/>
+      <c r="G70" s="51"/>
       <c r="H70" s="39">
         <v>6</v>
       </c>
       <c r="I70" s="33"/>
     </row>
-    <row r="71" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="40">
         <v>46</v>
       </c>
@@ -3244,7 +3387,7 @@
       </c>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="40">
         <v>47</v>
       </c>
@@ -3262,23 +3405,23 @@
       </c>
       <c r="I72" s="33"/>
     </row>
-    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="40"/>
       <c r="C73" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D73" s="36"/>
       <c r="E73" s="37"/>
-      <c r="F73" s="59" t="s">
+      <c r="F73" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="59"/>
+      <c r="G73" s="51"/>
       <c r="H73" s="39">
         <v>11</v>
       </c>
       <c r="I73" s="33"/>
     </row>
-    <row r="74" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="40">
         <v>48</v>
       </c>
@@ -3296,7 +3439,7 @@
       </c>
       <c r="I74" s="33"/>
     </row>
-    <row r="75" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="44">
         <v>49</v>
       </c>
@@ -3316,32 +3459,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F64:G64"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E20">
@@ -3362,9 +3505,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3384,9 +3527,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
second sprint choose task
</commit_message>
<xml_diff>
--- a/Doc/backlog-template.xlsx
+++ b/Doc/backlog-template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\Documents\GitHub\Ask_service\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -36,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="141">
   <si>
     <t>Kokhanov, Yeremenko, Tkachov, Daubur, Danilenko, Kiparenko, Golubchikov</t>
   </si>
@@ -1102,24 +1107,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1132,6 +1119,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1782,6 +1787,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2040,7 +2189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2051,8 +2200,8 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2071,50 +2220,50 @@
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -2166,10 +2315,10 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="55"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="15">
         <v>10</v>
       </c>
@@ -2251,10 +2400,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="23">
         <v>20</v>
       </c>
@@ -2354,10 +2503,10 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="23">
         <v>4</v>
       </c>
@@ -2419,10 +2568,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="56"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="23">
         <v>8</v>
       </c>
@@ -2484,10 +2633,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="56"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="23">
         <v>8</v>
       </c>
@@ -2542,10 +2691,10 @@
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="23">
         <v>8</v>
       </c>
@@ -2594,10 +2743,10 @@
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="54" t="s">
+      <c r="F27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="58"/>
       <c r="H27" s="23">
         <v>13</v>
       </c>
@@ -2608,7 +2757,9 @@
         <v>16</v>
       </c>
       <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
+      <c r="D28" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="E28" s="30"/>
       <c r="F28" s="32" t="s">
         <v>54</v>
@@ -2646,10 +2797,10 @@
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="54" t="s">
+      <c r="F30" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="23">
         <v>12</v>
       </c>
@@ -2734,10 +2885,10 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="54" t="s">
+      <c r="F35" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="23">
         <v>11</v>
       </c>
@@ -2788,10 +2939,10 @@
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="54" t="s">
+      <c r="F38" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="54"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="23">
         <v>18</v>
       </c>
@@ -2880,10 +3031,10 @@
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="51" t="s">
+      <c r="F43" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="G43" s="51"/>
+      <c r="G43" s="59"/>
       <c r="H43" s="23">
         <v>11</v>
       </c>
@@ -2952,10 +3103,10 @@
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="37"/>
-      <c r="F47" s="53" t="s">
+      <c r="F47" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="53"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="39">
         <v>6</v>
       </c>
@@ -3028,10 +3179,10 @@
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="37"/>
-      <c r="F51" s="51" t="s">
+      <c r="F51" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="51"/>
+      <c r="G51" s="59"/>
       <c r="H51" s="39">
         <v>5</v>
       </c>
@@ -3062,10 +3213,10 @@
       </c>
       <c r="D53" s="36"/>
       <c r="E53" s="37"/>
-      <c r="F53" s="51" t="s">
+      <c r="F53" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="G53" s="51"/>
+      <c r="G53" s="59"/>
       <c r="H53" s="39">
         <v>7</v>
       </c>
@@ -3114,10 +3265,10 @@
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="37"/>
-      <c r="F56" s="51" t="s">
+      <c r="F56" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="51"/>
+      <c r="G56" s="59"/>
       <c r="H56" s="39">
         <v>10</v>
       </c>
@@ -3166,10 +3317,10 @@
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="37"/>
-      <c r="F59" s="52" t="s">
+      <c r="F59" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="52"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="39">
         <v>4</v>
       </c>
@@ -3222,10 +3373,10 @@
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="37"/>
-      <c r="F62" s="51" t="s">
+      <c r="F62" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="51"/>
+      <c r="G62" s="59"/>
       <c r="H62" s="39">
         <v>5</v>
       </c>
@@ -3256,10 +3407,10 @@
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="37"/>
-      <c r="F64" s="51" t="s">
+      <c r="F64" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="G64" s="51"/>
+      <c r="G64" s="59"/>
       <c r="H64" s="39">
         <v>8</v>
       </c>
@@ -3326,10 +3477,10 @@
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="37"/>
-      <c r="F68" s="51" t="s">
+      <c r="F68" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="G68" s="51"/>
+      <c r="G68" s="59"/>
       <c r="H68" s="39">
         <v>3</v>
       </c>
@@ -3360,10 +3511,10 @@
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="37"/>
-      <c r="F70" s="51" t="s">
+      <c r="F70" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="51"/>
+      <c r="G70" s="59"/>
       <c r="H70" s="39">
         <v>6</v>
       </c>
@@ -3412,10 +3563,10 @@
       </c>
       <c r="D73" s="36"/>
       <c r="E73" s="37"/>
-      <c r="F73" s="51" t="s">
+      <c r="F73" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="51"/>
+      <c r="G73" s="59"/>
       <c r="H73" s="39">
         <v>11</v>
       </c>
@@ -3459,32 +3610,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F64:G64"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E20">

</xml_diff>

<commit_message>
Change my task for 2 sprint
Changed task
</commit_message>
<xml_diff>
--- a/Doc/backlog-template.xlsx
+++ b/Doc/backlog-template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
@@ -504,8 +504,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1105,6 +1105,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1117,24 +1135,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1785,6 +1785,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2043,22 +2187,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.85546875"/>
     <col min="2" max="2" width="6.28515625"/>
@@ -2072,56 +2216,56 @@
     <col min="10" max="10" width="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39" customHeight="1">
+    <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2134,7 +2278,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="15">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2161,7 +2305,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="23.25" customHeight="1">
+    <row r="6" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
@@ -2169,17 +2313,17 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="15">
         <v>10</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1">
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="17">
         <v>1</v>
@@ -2202,7 +2346,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1">
+    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="17">
         <v>2</v>
@@ -2225,7 +2369,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="17">
         <v>3</v>
@@ -2246,7 +2390,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1">
+    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
@@ -2254,10 +2398,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="57"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="23">
         <v>20</v>
       </c>
@@ -2265,7 +2409,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="39" customHeight="1">
+    <row r="11" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="17">
         <v>4</v>
@@ -2288,7 +2432,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="37.5" customHeight="1">
+    <row r="12" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="17">
         <v>5</v>
@@ -2311,7 +2455,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="38.25" customHeight="1">
+    <row r="13" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="17">
         <v>6</v>
@@ -2332,7 +2476,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="38.25" customHeight="1">
+    <row r="14" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="17">
         <v>7</v>
@@ -2353,7 +2497,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="24" customHeight="1">
+    <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
@@ -2361,10 +2505,10 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="57"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="23">
         <v>4</v>
       </c>
@@ -2372,7 +2516,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="24" customHeight="1">
+    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="17">
         <v>8</v>
@@ -2395,7 +2539,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="39" customHeight="1">
+    <row r="17" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="17">
         <v>9</v>
@@ -2418,7 +2562,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="24" customHeight="1">
+    <row r="18" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
@@ -2426,10 +2570,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="57"/>
+      <c r="G18" s="56"/>
       <c r="H18" s="23">
         <v>8</v>
       </c>
@@ -2437,7 +2581,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="47.25" customHeight="1">
+    <row r="19" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="17">
         <v>10</v>
@@ -2460,7 +2604,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="39.75" customHeight="1">
+    <row r="20" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="17">
         <v>11</v>
@@ -2483,7 +2627,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="24" customHeight="1">
+    <row r="21" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
@@ -2491,10 +2635,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="57"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="23">
         <v>8</v>
       </c>
@@ -2502,7 +2646,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="40.5" customHeight="1">
+    <row r="22" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <v>12</v>
       </c>
@@ -2522,7 +2666,7 @@
       </c>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" spans="1:11" ht="38.25" customHeight="1">
+    <row r="23" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <v>13</v>
       </c>
@@ -2542,23 +2686,23 @@
       </c>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="1:11" ht="38.25" customHeight="1">
+    <row r="24" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="58" t="s">
+      <c r="F24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="58"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="23">
         <v>8</v>
       </c>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="1:11" ht="43.15" customHeight="1">
+    <row r="25" spans="1:11" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <v>14</v>
       </c>
@@ -2576,7 +2720,7 @@
       </c>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="1:11" ht="45" customHeight="1">
+    <row r="26" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>15</v>
       </c>
@@ -2594,23 +2738,23 @@
       </c>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="58" t="s">
+      <c r="F27" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="58"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="23">
         <v>13</v>
       </c>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="1:11" ht="32.450000000000003" customHeight="1">
+    <row r="28" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17">
         <v>16</v>
       </c>
@@ -2628,7 +2772,7 @@
       </c>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="1:11" ht="31.15" customHeight="1">
+    <row r="29" spans="1:11" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <v>17</v>
       </c>
@@ -2646,23 +2790,23 @@
       </c>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1">
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="58" t="s">
+      <c r="F30" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="58"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="23">
         <v>12</v>
       </c>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" spans="1:11" ht="47.45" customHeight="1">
+    <row r="31" spans="1:11" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17">
         <v>18</v>
       </c>
@@ -2680,7 +2824,7 @@
       </c>
       <c r="I31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="54.6" customHeight="1">
+    <row r="32" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17">
         <v>19</v>
       </c>
@@ -2698,7 +2842,7 @@
       </c>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" spans="2:9" ht="46.15" customHeight="1">
+    <row r="33" spans="2:9" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17">
         <v>20</v>
       </c>
@@ -2716,7 +2860,7 @@
       </c>
       <c r="I33" s="33"/>
     </row>
-    <row r="34" spans="2:9" ht="46.9" customHeight="1">
+    <row r="34" spans="2:9" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
         <v>21</v>
       </c>
@@ -2734,23 +2878,23 @@
       </c>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" spans="2:9" ht="15" customHeight="1">
+    <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="58" t="s">
+      <c r="F35" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="58"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="23">
         <v>11</v>
       </c>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" spans="2:9" ht="47.45" customHeight="1">
+    <row r="36" spans="2:9" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17">
         <v>22</v>
       </c>
@@ -2770,7 +2914,7 @@
       </c>
       <c r="I36" s="33"/>
     </row>
-    <row r="37" spans="2:9" ht="30.6" customHeight="1">
+    <row r="37" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
         <v>23</v>
       </c>
@@ -2788,23 +2932,23 @@
       </c>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" spans="2:9" ht="15" customHeight="1">
+    <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
       <c r="C38" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="58" t="s">
+      <c r="F38" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="58"/>
+      <c r="G38" s="54"/>
       <c r="H38" s="23">
         <v>18</v>
       </c>
       <c r="I38" s="33"/>
     </row>
-    <row r="39" spans="2:9" ht="43.15" customHeight="1">
+    <row r="39" spans="2:9" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
         <v>24</v>
       </c>
@@ -2822,14 +2966,12 @@
       </c>
       <c r="I39" s="33"/>
     </row>
-    <row r="40" spans="2:9" ht="31.9" customHeight="1">
+    <row r="40" spans="2:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="17">
         <v>25</v>
       </c>
       <c r="C40" s="28"/>
-      <c r="D40" s="29" t="s">
-        <v>14</v>
-      </c>
+      <c r="D40" s="29"/>
       <c r="E40" s="30"/>
       <c r="F40" s="31" t="s">
         <v>75</v>
@@ -2842,7 +2984,7 @@
       </c>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" spans="2:9" ht="57" customHeight="1">
+    <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="17">
         <v>26</v>
       </c>
@@ -2862,7 +3004,7 @@
       </c>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" spans="2:9" ht="91.5" customHeight="1">
+    <row r="42" spans="2:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="17">
         <v>27</v>
       </c>
@@ -2880,23 +3022,23 @@
       </c>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" spans="2:9" ht="15" customHeight="1">
+    <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
       <c r="C43" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="59" t="s">
+      <c r="F43" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="G43" s="59"/>
+      <c r="G43" s="51"/>
       <c r="H43" s="23">
         <v>11</v>
       </c>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" spans="2:9" ht="42" customHeight="1">
+    <row r="44" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="17">
         <v>28</v>
       </c>
@@ -2914,7 +3056,7 @@
       </c>
       <c r="I44" s="33"/>
     </row>
-    <row r="45" spans="2:9" ht="58.5" customHeight="1">
+    <row r="45" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="17">
         <v>29</v>
       </c>
@@ -2932,7 +3074,7 @@
       </c>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" spans="2:9" ht="28.5" customHeight="1">
+    <row r="46" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17">
         <v>30</v>
       </c>
@@ -2952,23 +3094,23 @@
       </c>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" spans="2:9" ht="15" customHeight="1">
+    <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="37"/>
-      <c r="F47" s="60" t="s">
+      <c r="F47" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="60"/>
+      <c r="G47" s="53"/>
       <c r="H47" s="39">
         <v>6</v>
       </c>
       <c r="I47" s="33"/>
     </row>
-    <row r="48" spans="2:9" ht="51.75" customHeight="1">
+    <row r="48" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="17">
         <v>31</v>
       </c>
@@ -2988,7 +3130,7 @@
       </c>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" spans="2:9" ht="50.25" customHeight="1">
+    <row r="49" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="17">
         <v>32</v>
       </c>
@@ -3008,7 +3150,7 @@
       </c>
       <c r="I49" s="33"/>
     </row>
-    <row r="50" spans="2:9" ht="46.5" customHeight="1">
+    <row r="50" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="40">
         <v>33</v>
       </c>
@@ -3028,23 +3170,23 @@
       </c>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" spans="2:9" ht="15" customHeight="1">
+    <row r="51" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="40"/>
       <c r="C51" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="37"/>
-      <c r="F51" s="59" t="s">
+      <c r="F51" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="59"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="39">
         <v>5</v>
       </c>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" spans="2:9" ht="53.25" customHeight="1">
+    <row r="52" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="40">
         <v>34</v>
       </c>
@@ -3062,28 +3204,30 @@
       </c>
       <c r="I52" s="33"/>
     </row>
-    <row r="53" spans="2:9" ht="15" customHeight="1">
+    <row r="53" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="40"/>
       <c r="C53" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D53" s="36"/>
       <c r="E53" s="37"/>
-      <c r="F53" s="59" t="s">
+      <c r="F53" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="G53" s="59"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="39">
         <v>7</v>
       </c>
       <c r="I53" s="33"/>
     </row>
-    <row r="54" spans="2:9" ht="43.5" customHeight="1">
+    <row r="54" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="40">
         <v>35</v>
       </c>
       <c r="C54" s="28"/>
-      <c r="D54" s="36"/>
+      <c r="D54" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="E54" s="37"/>
       <c r="F54" s="42" t="s">
         <v>101</v>
@@ -3096,7 +3240,7 @@
       </c>
       <c r="I54" s="33"/>
     </row>
-    <row r="55" spans="2:9" ht="48" customHeight="1">
+    <row r="55" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="40">
         <v>36</v>
       </c>
@@ -3114,23 +3258,23 @@
       </c>
       <c r="I55" s="33"/>
     </row>
-    <row r="56" spans="2:9" ht="15" customHeight="1">
+    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="40"/>
       <c r="C56" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="37"/>
-      <c r="F56" s="59" t="s">
+      <c r="F56" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="59"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="39">
         <v>10</v>
       </c>
       <c r="I56" s="33"/>
     </row>
-    <row r="57" spans="2:9" ht="33.75" customHeight="1">
+    <row r="57" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="40">
         <v>37</v>
       </c>
@@ -3148,7 +3292,7 @@
       </c>
       <c r="I57" s="33"/>
     </row>
-    <row r="58" spans="2:9" ht="29.25" customHeight="1">
+    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="40">
         <v>38</v>
       </c>
@@ -3166,23 +3310,23 @@
       </c>
       <c r="I58" s="33"/>
     </row>
-    <row r="59" spans="2:9" ht="15" customHeight="1">
+    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="40"/>
       <c r="C59" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="37"/>
-      <c r="F59" s="61" t="s">
+      <c r="F59" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="61"/>
+      <c r="G59" s="52"/>
       <c r="H59" s="39">
         <v>4</v>
       </c>
       <c r="I59" s="33"/>
     </row>
-    <row r="60" spans="2:9" ht="34.5" customHeight="1">
+    <row r="60" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="40">
         <v>39</v>
       </c>
@@ -3202,7 +3346,7 @@
       </c>
       <c r="I60" s="33"/>
     </row>
-    <row r="61" spans="2:9" ht="32.25" customHeight="1">
+    <row r="61" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="40">
         <v>40</v>
       </c>
@@ -3222,23 +3366,23 @@
       </c>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="2:9" ht="15" customHeight="1">
+    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="40"/>
       <c r="C62" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="37"/>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="59"/>
+      <c r="G62" s="51"/>
       <c r="H62" s="39">
         <v>5</v>
       </c>
       <c r="I62" s="33"/>
     </row>
-    <row r="63" spans="2:9" ht="38.25" customHeight="1">
+    <row r="63" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="40">
         <v>41</v>
       </c>
@@ -3256,23 +3400,23 @@
       </c>
       <c r="I63" s="33"/>
     </row>
-    <row r="64" spans="2:9" ht="15" customHeight="1">
+    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="40"/>
       <c r="C64" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="37"/>
-      <c r="F64" s="59" t="s">
+      <c r="F64" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="G64" s="59"/>
+      <c r="G64" s="51"/>
       <c r="H64" s="39">
         <v>8</v>
       </c>
       <c r="I64" s="33"/>
     </row>
-    <row r="65" spans="2:9" ht="48.75" customHeight="1">
+    <row r="65" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="40">
         <v>42</v>
       </c>
@@ -3290,7 +3434,7 @@
       </c>
       <c r="I65" s="33"/>
     </row>
-    <row r="66" spans="2:9" ht="33" customHeight="1">
+    <row r="66" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="40">
         <v>43</v>
       </c>
@@ -3308,7 +3452,7 @@
       </c>
       <c r="I66" s="33"/>
     </row>
-    <row r="67" spans="2:9" ht="30.75" customHeight="1">
+    <row r="67" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="40">
         <v>44</v>
       </c>
@@ -3326,23 +3470,23 @@
       </c>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1">
+    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="40"/>
       <c r="C68" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="37"/>
-      <c r="F68" s="59" t="s">
+      <c r="F68" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="G68" s="59"/>
+      <c r="G68" s="51"/>
       <c r="H68" s="39">
         <v>3</v>
       </c>
       <c r="I68" s="33"/>
     </row>
-    <row r="69" spans="2:9" ht="44.25" customHeight="1">
+    <row r="69" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="40">
         <v>45</v>
       </c>
@@ -3360,23 +3504,23 @@
       </c>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="2:9" ht="15" customHeight="1">
+    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="40"/>
       <c r="C70" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="37"/>
-      <c r="F70" s="59" t="s">
+      <c r="F70" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="59"/>
+      <c r="G70" s="51"/>
       <c r="H70" s="39">
         <v>6</v>
       </c>
       <c r="I70" s="33"/>
     </row>
-    <row r="71" spans="2:9" ht="36" customHeight="1">
+    <row r="71" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="40">
         <v>46</v>
       </c>
@@ -3394,7 +3538,7 @@
       </c>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" spans="2:9" ht="53.25" customHeight="1">
+    <row r="72" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="40">
         <v>47</v>
       </c>
@@ -3412,23 +3556,23 @@
       </c>
       <c r="I72" s="33"/>
     </row>
-    <row r="73" spans="2:9" ht="15" customHeight="1">
+    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="40"/>
       <c r="C73" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D73" s="36"/>
       <c r="E73" s="37"/>
-      <c r="F73" s="59" t="s">
+      <c r="F73" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="59"/>
+      <c r="G73" s="51"/>
       <c r="H73" s="39">
         <v>11</v>
       </c>
       <c r="I73" s="33"/>
     </row>
-    <row r="74" spans="2:9" ht="43.5" customHeight="1">
+    <row r="74" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="40">
         <v>48</v>
       </c>
@@ -3446,7 +3590,7 @@
       </c>
       <c r="I74" s="33"/>
     </row>
-    <row r="75" spans="2:9" ht="53.25" customHeight="1">
+    <row r="75" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="44">
         <v>49</v>
       </c>
@@ -3466,32 +3610,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F64:G64"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E20">
@@ -3507,14 +3651,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3529,14 +3673,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
My tasks for second sprint
My tasks for second sprint
</commit_message>
<xml_diff>
--- a/Doc/backlog-template.xlsx
+++ b/Doc/backlog-template.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="142">
   <si>
     <t>Kokhanov, Yeremenko, Tkachov, Daubur, Danilenko, Kiparenko, Golubchikov</t>
   </si>
@@ -1105,24 +1105,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1135,6 +1117,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1929,6 +1929,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2187,7 +2331,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2198,8 +2342,8 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2218,50 +2362,50 @@
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -2313,10 +2457,10 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="55"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="15">
         <v>10</v>
       </c>
@@ -2398,10 +2542,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="23">
         <v>20</v>
       </c>
@@ -2505,10 +2649,10 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="23">
         <v>4</v>
       </c>
@@ -2570,10 +2714,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="56"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="23">
         <v>8</v>
       </c>
@@ -2635,10 +2779,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="56"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="23">
         <v>8</v>
       </c>
@@ -2693,10 +2837,10 @@
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="23">
         <v>8</v>
       </c>
@@ -2745,10 +2889,10 @@
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="54" t="s">
+      <c r="F27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="58"/>
       <c r="H27" s="23">
         <v>13</v>
       </c>
@@ -2797,10 +2941,10 @@
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="54" t="s">
+      <c r="F30" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="23">
         <v>12</v>
       </c>
@@ -2885,10 +3029,10 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="54" t="s">
+      <c r="F35" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="23">
         <v>11</v>
       </c>
@@ -2919,7 +3063,9 @@
         <v>23</v>
       </c>
       <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
+      <c r="D37" s="29" t="s">
+        <v>137</v>
+      </c>
       <c r="E37" s="30"/>
       <c r="F37" s="31" t="s">
         <v>70</v>
@@ -2939,10 +3085,10 @@
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="54" t="s">
+      <c r="F38" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="54"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="23">
         <v>18</v>
       </c>
@@ -2971,7 +3117,9 @@
         <v>25</v>
       </c>
       <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
+      <c r="D40" s="29" t="s">
+        <v>137</v>
+      </c>
       <c r="E40" s="30"/>
       <c r="F40" s="31" t="s">
         <v>75</v>
@@ -3009,7 +3157,9 @@
         <v>27</v>
       </c>
       <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
+      <c r="D42" s="29" t="s">
+        <v>137</v>
+      </c>
       <c r="E42" s="30"/>
       <c r="F42" s="34" t="s">
         <v>79</v>
@@ -3029,10 +3179,10 @@
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="51" t="s">
+      <c r="F43" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="G43" s="51"/>
+      <c r="G43" s="59"/>
       <c r="H43" s="23">
         <v>11</v>
       </c>
@@ -3101,10 +3251,10 @@
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="37"/>
-      <c r="F47" s="53" t="s">
+      <c r="F47" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="53"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="39">
         <v>6</v>
       </c>
@@ -3177,10 +3327,10 @@
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="37"/>
-      <c r="F51" s="51" t="s">
+      <c r="F51" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="51"/>
+      <c r="G51" s="59"/>
       <c r="H51" s="39">
         <v>5</v>
       </c>
@@ -3211,10 +3361,10 @@
       </c>
       <c r="D53" s="36"/>
       <c r="E53" s="37"/>
-      <c r="F53" s="51" t="s">
+      <c r="F53" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="G53" s="51"/>
+      <c r="G53" s="59"/>
       <c r="H53" s="39">
         <v>7</v>
       </c>
@@ -3265,10 +3415,10 @@
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="37"/>
-      <c r="F56" s="51" t="s">
+      <c r="F56" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="51"/>
+      <c r="G56" s="59"/>
       <c r="H56" s="39">
         <v>10</v>
       </c>
@@ -3317,10 +3467,10 @@
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="37"/>
-      <c r="F59" s="52" t="s">
+      <c r="F59" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="52"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="39">
         <v>4</v>
       </c>
@@ -3373,10 +3523,10 @@
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="37"/>
-      <c r="F62" s="51" t="s">
+      <c r="F62" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="51"/>
+      <c r="G62" s="59"/>
       <c r="H62" s="39">
         <v>5</v>
       </c>
@@ -3407,10 +3557,10 @@
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="37"/>
-      <c r="F64" s="51" t="s">
+      <c r="F64" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="G64" s="51"/>
+      <c r="G64" s="59"/>
       <c r="H64" s="39">
         <v>8</v>
       </c>
@@ -3477,10 +3627,10 @@
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="37"/>
-      <c r="F68" s="51" t="s">
+      <c r="F68" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="G68" s="51"/>
+      <c r="G68" s="59"/>
       <c r="H68" s="39">
         <v>3</v>
       </c>
@@ -3511,10 +3661,10 @@
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="37"/>
-      <c r="F70" s="51" t="s">
+      <c r="F70" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="51"/>
+      <c r="G70" s="59"/>
       <c r="H70" s="39">
         <v>6</v>
       </c>
@@ -3563,10 +3713,10 @@
       </c>
       <c r="D73" s="36"/>
       <c r="E73" s="37"/>
-      <c r="F73" s="51" t="s">
+      <c r="F73" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="51"/>
+      <c r="G73" s="59"/>
       <c r="H73" s="39">
         <v>11</v>
       </c>
@@ -3610,32 +3760,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F64:G64"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E20">

</xml_diff>

<commit_message>
Ready Sprint Backlogs and Burndown Chat Diagrams
Remake of 1 and 2 Sprint Backlogs, added 3 and 4 Sprint Backlogs(with
Burndown Chat Diagrams inside these files)
</commit_message>
<xml_diff>
--- a/Doc/backlog-template.xlsx
+++ b/Doc/backlog-template.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
   <si>
     <t>Kokhanov, Yeremenko, Tkachov, Daubur, Danilenko, Kiparenko, Golubchikov</t>
   </si>
@@ -114,33 +114,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>As an unregistered user, I want to browse users' pages</t>
-  </si>
-  <si>
-    <t>Valera</t>
-  </si>
-  <si>
-    <t>Implement, choose registered user</t>
-  </si>
-  <si>
-    <t>I choose a registered user and clicking on its icon turn on his page</t>
-  </si>
-  <si>
-    <t>Implement, browse registered user`s wall</t>
-  </si>
-  <si>
     <t>I look through the wall will register the user box on his page</t>
   </si>
   <si>
-    <t>Implement, browse registered user`s profile, if it is not hidden</t>
-  </si>
-  <si>
     <t>If the page the user is not hidden, I can see all the information about the user and his wall with questions</t>
   </si>
   <si>
-    <t>As an unregistered user, I want to authorize from my other social network accounts</t>
-  </si>
-  <si>
     <t>Implement, authorize from vk.com</t>
   </si>
   <si>
@@ -159,18 +138,9 @@
     <t>To login to the site I can use the social network twitter.com clicking on the appropriate button for the icon of the social network</t>
   </si>
   <si>
-    <t>Implement, authorize from myspace.com</t>
-  </si>
-  <si>
     <t>To login to the site I can use a social network myspace.com clicking on the appropriate button for the icon of the social network</t>
   </si>
   <si>
-    <t>As an unregistered user, I want to register through the website</t>
-  </si>
-  <si>
-    <t>Dima</t>
-  </si>
-  <si>
     <t>Create, textbox for registred login  and password</t>
   </si>
   <si>
@@ -183,12 +153,6 @@
     <t>In the appropriate fields when registering to enter your name, surname, age, date of birth for display on the main page.</t>
   </si>
   <si>
-    <t>As an unregistered user, I want to send anonimus questions to registerd users</t>
-  </si>
-  <si>
-    <t>Jenya</t>
-  </si>
-  <si>
     <t>Implement, question special box on a user`s wall</t>
   </si>
   <si>
@@ -204,9 +168,6 @@
     <t>As a registred user, I want to choose message sending mode</t>
   </si>
   <si>
-    <t>Sergey</t>
-  </si>
-  <si>
     <t>Implement, checkbox for choose anonimus message sending  mode</t>
   </si>
   <si>
@@ -252,57 +213,30 @@
     <t>As a registred user, I want to attach my social network accounts</t>
   </si>
   <si>
-    <t>As a registered user, I want to attach vk.com account</t>
-  </si>
-  <si>
     <t>In the settings of your account by clicking on the icon in the social network vk.com can attach your account with a social network</t>
   </si>
   <si>
-    <t>As a registered user, I want to attach facebook.com account</t>
-  </si>
-  <si>
     <t>In the settings of your account by clicking on the icon of the social network facebook.com, you can attach your account with a social network</t>
   </si>
   <si>
-    <t>As a registered user, I want to attach myspace.com account</t>
-  </si>
-  <si>
     <t>In the settings of your account by clicking on the icon of a social network myspace.com you can attach your account with a social network</t>
   </si>
   <si>
-    <t>As a registered user, I want to attach twitter.com account</t>
-  </si>
-  <si>
     <t>In the settings of your account by clicking on the icon in the social network twitter.com you can attach your account with a social network</t>
   </si>
   <si>
-    <t>As a registered user, I want to control my friendlist</t>
-  </si>
-  <si>
-    <t>As a registered user, I want to add a registerd user to my friendlist</t>
-  </si>
-  <si>
     <t>Being on the other page and clicking on the "Add as friend" button, you can add this user to your friends list</t>
   </si>
   <si>
-    <t>As a rsuser, I want to delete a registerd user to my friendlist</t>
-  </si>
-  <si>
     <t>When you click on the delete button opposite to each other in the friends list, you can delete it from the list</t>
   </si>
   <si>
     <t>As a registred user, I want to control my profile</t>
   </si>
   <si>
-    <t>As a registered user, I want to  change background of my page</t>
-  </si>
-  <si>
     <t>In the settings of your page I can choose the background, different, or upload an image from your computer and use it as a background</t>
   </si>
   <si>
-    <t>As a registered user, I want to  add my mude to my page</t>
-  </si>
-  <si>
     <t>I can add status to your page that will be displayed on my page</t>
   </si>
   <si>
@@ -333,9 +267,6 @@
     <t>To do this, click on the question, the display for the answer to the question, for the answer to another question, repeat the operation</t>
   </si>
   <si>
-    <t>Kirill</t>
-  </si>
-  <si>
     <t>write an answer on chosen question</t>
   </si>
   <si>
@@ -345,9 +276,6 @@
     <t>As a registred user, I want to get statistic information about my account</t>
   </si>
   <si>
-    <t>Kiparenko</t>
-  </si>
-  <si>
     <t>view number of my answers</t>
   </si>
   <si>
@@ -366,9 +294,6 @@
     <t>To see the number of responses, you need to look in the "Liked" in the upper right corner at the beginning of the wall</t>
   </si>
   <si>
-    <t>As a registred user, I want to follow registered users` pages</t>
-  </si>
-  <si>
     <t>follow the page, I am interested in</t>
   </si>
   <si>
@@ -390,24 +315,12 @@
     <t>After filling out the field for a comment you need to press the "Add Comment", which will add a comment</t>
   </si>
   <si>
-    <t>As a user, I want to search registered users` pages</t>
-  </si>
-  <si>
-    <t>search registered users` pages by keywords</t>
-  </si>
-  <si>
     <t>The search string is entered at which a word search</t>
   </si>
   <si>
-    <t>filter the list of registered users` pages</t>
-  </si>
-  <si>
     <t>Filtration is carried out in the fields selected by the user</t>
   </si>
   <si>
-    <t>As a user, I want to send questions to registered users</t>
-  </si>
-  <si>
     <t>input my question on user`s page wall</t>
   </si>
   <si>
@@ -486,9 +399,6 @@
     <t>To write warning comes on the admin page, you need a user clicks on the desired content, clicks on the "Warning" in the box that appears, writes the warning text</t>
   </si>
   <si>
-    <t>Igor</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -498,14 +408,80 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Evgeniy</t>
+    <t>As a user, I want to delete a registred user to my friendlist</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to control my friendlist</t>
+  </si>
+  <si>
+    <t>As an unregistred user, I want to browse users' pages</t>
+  </si>
+  <si>
+    <t>Implement, choose registred user</t>
+  </si>
+  <si>
+    <t>I choose a registred user and clicking on its icon turn on his page</t>
+  </si>
+  <si>
+    <t>Implement, browse registred user`s wall</t>
+  </si>
+  <si>
+    <t>Implement, browse registred user`s profile, if it is not hidden</t>
+  </si>
+  <si>
+    <t>As an unregistred user, I want to authorize from my other social network accounts</t>
+  </si>
+  <si>
+    <t>As an unregistred user, I want to register through the website</t>
+  </si>
+  <si>
+    <t>As an unregistred user, I want to send anonimus questions to registerd users</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to attach vk.com account</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to attach facebook.com account</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to attach twitter.com account</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to add a registred user to my friendlist</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to  change background of my page</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to  add my mude to my page</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to follow registred users` pages</t>
+  </si>
+  <si>
+    <t>As a user, I want to search registred users` pages</t>
+  </si>
+  <si>
+    <t>search registred users` pages by keywords</t>
+  </si>
+  <si>
+    <t>filter the list of registred users` pages</t>
+  </si>
+  <si>
+    <t>As a user, I want to send questions to registred users</t>
+  </si>
+  <si>
+    <t>Implement, authorize from Google+</t>
+  </si>
+  <si>
+    <t>As a registred user, I want to attach Google+ account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -588,8 +564,16 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +596,48 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -963,7 +989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1015,27 +1041,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1045,45 +1056,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1094,9 +1081,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,23 +1102,137 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2073,6 +2171,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2331,7 +2573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2342,8 +2584,8 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6:G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2362,50 +2604,50 @@
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -2453,14 +2695,14 @@
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="56"/>
+      <c r="F6" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="65"/>
       <c r="H6" s="15">
         <v>10</v>
       </c>
@@ -2473,20 +2715,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="23">
+      <c r="F7" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="21">
         <v>2</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
@@ -2496,20 +2736,18 @@
         <v>2</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="D8" s="19"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="23">
+      <c r="F8" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="21">
         <v>5</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
     </row>
@@ -2521,16 +2759,16 @@
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="23">
+      <c r="F9" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="21">
         <v>3</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
     </row>
@@ -2538,18 +2776,18 @@
       <c r="A10" s="2"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="57"/>
-      <c r="H10" s="23">
+      <c r="F10" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="68"/>
+      <c r="H10" s="21">
         <v>20</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
     </row>
@@ -2559,20 +2797,18 @@
         <v>4</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="19" t="s">
-        <v>141</v>
-      </c>
+      <c r="D11" s="19"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="23">
+      <c r="F11" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="21">
         <v>5</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="22"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
     </row>
@@ -2582,20 +2818,18 @@
         <v>5</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="19" t="s">
-        <v>141</v>
-      </c>
+      <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="23">
+      <c r="F12" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="21">
         <v>5</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="22"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
     </row>
@@ -2607,16 +2841,16 @@
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="23">
+      <c r="F13" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="21">
         <v>5</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="22"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
     </row>
@@ -2628,16 +2862,16 @@
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="23">
+      <c r="F14" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="21">
         <v>5</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
     </row>
@@ -2645,18 +2879,18 @@
       <c r="A15" s="2"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="23">
+      <c r="F15" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="46"/>
+      <c r="H15" s="21">
         <v>4</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
     </row>
@@ -2666,20 +2900,18 @@
         <v>8</v>
       </c>
       <c r="C16" s="18"/>
-      <c r="D16" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="D16" s="19"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="23">
+      <c r="F16" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="21">
         <v>1</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
     </row>
@@ -2689,20 +2921,18 @@
         <v>9</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="D17" s="19"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="23">
+      <c r="F17" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="21">
         <v>3</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
     </row>
@@ -2710,18 +2940,18 @@
       <c r="A18" s="2"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="23">
+      <c r="F18" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="68"/>
+      <c r="H18" s="21">
         <v>8</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
     </row>
@@ -2731,20 +2961,18 @@
         <v>10</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="D19" s="19"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="23">
+      <c r="F19" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="21">
         <v>5</v>
       </c>
-      <c r="I19" s="24"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
     </row>
@@ -2754,20 +2982,18 @@
         <v>11</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="D20" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="D20" s="19"/>
       <c r="E20" s="20"/>
-      <c r="F20" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="23">
+      <c r="F20" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="21">
         <v>3</v>
       </c>
-      <c r="I20" s="24"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
     </row>
@@ -2775,18 +3001,18 @@
       <c r="A21" s="2"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="23">
+      <c r="F21" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="21">
         <v>8</v>
       </c>
-      <c r="I21" s="24"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
     </row>
@@ -2794,998 +3020,970 @@
       <c r="B22" s="17">
         <v>12</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="23">
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="21">
         <v>5</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <v>13</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="23">
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="21">
         <v>3</v>
       </c>
-      <c r="I23" s="33"/>
+      <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
-      <c r="C24" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="58"/>
-      <c r="H24" s="23">
+      <c r="C24" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="48"/>
+      <c r="H24" s="21">
         <v>8</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <v>14</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" s="23">
+      <c r="C25" s="23"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="21">
         <v>3</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>15</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="23">
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="21">
         <v>5</v>
       </c>
-      <c r="I26" s="33"/>
+      <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
-      <c r="C27" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="58"/>
-      <c r="H27" s="23">
+      <c r="C27" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="62"/>
+      <c r="H27" s="21">
         <v>13</v>
       </c>
-      <c r="I27" s="33"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17">
         <v>16</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="23">
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="21">
         <v>8</v>
       </c>
-      <c r="I28" s="33"/>
+      <c r="I28" s="26"/>
     </row>
     <row r="29" spans="1:11" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <v>17</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="H29" s="23">
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="21">
         <v>5</v>
       </c>
-      <c r="I29" s="33"/>
+      <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
-      <c r="C30" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="58"/>
-      <c r="H30" s="23">
+      <c r="C30" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="59"/>
+      <c r="H30" s="21">
         <v>12</v>
       </c>
-      <c r="I30" s="33"/>
+      <c r="I30" s="26"/>
     </row>
     <row r="31" spans="1:11" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17">
         <v>18</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="23">
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="21">
         <v>3</v>
       </c>
-      <c r="I31" s="33"/>
+      <c r="I31" s="26"/>
     </row>
     <row r="32" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17">
         <v>19</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" s="23">
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="21">
         <v>3</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="26"/>
     </row>
     <row r="33" spans="2:9" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17">
         <v>20</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="23">
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="21">
         <v>3</v>
       </c>
-      <c r="I33" s="33"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="2:9" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
         <v>21</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" s="23">
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="21">
         <v>3</v>
       </c>
-      <c r="I34" s="33"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
-      <c r="C35" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="58"/>
-      <c r="H35" s="23">
+      <c r="C35" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="74"/>
+      <c r="H35" s="21">
         <v>11</v>
       </c>
-      <c r="I35" s="33"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="2:9" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17">
         <v>22</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="23">
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="21">
         <v>8</v>
       </c>
-      <c r="I36" s="33"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="2:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
         <v>23</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="H37" s="23">
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="21">
         <v>3</v>
       </c>
-      <c r="I37" s="33"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
-      <c r="C38" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="58"/>
-      <c r="H38" s="23">
+      <c r="C38" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="59"/>
+      <c r="H38" s="21">
         <v>18</v>
       </c>
-      <c r="I38" s="33"/>
+      <c r="I38" s="26"/>
     </row>
     <row r="39" spans="2:9" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
         <v>24</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="H39" s="23">
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="21">
         <v>8</v>
       </c>
-      <c r="I39" s="33"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="2:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="17">
         <v>25</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="H40" s="23">
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="21">
         <v>2</v>
       </c>
-      <c r="I40" s="33"/>
+      <c r="I40" s="26"/>
     </row>
     <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="17">
         <v>26</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="H41" s="23">
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="21">
         <v>5</v>
       </c>
-      <c r="I41" s="33"/>
+      <c r="I41" s="26"/>
     </row>
     <row r="42" spans="2:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="17">
         <v>27</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="H42" s="23">
+      <c r="C42" s="23"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="21">
         <v>3</v>
       </c>
-      <c r="I42" s="33"/>
+      <c r="I42" s="26"/>
     </row>
     <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
-      <c r="C43" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="59"/>
-      <c r="H43" s="23">
+      <c r="C43" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="G43" s="52"/>
+      <c r="H43" s="21">
         <v>11</v>
       </c>
-      <c r="I43" s="33"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="17">
         <v>28</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="G44" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="39">
+      <c r="C44" s="23"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H44" s="29">
         <v>5</v>
       </c>
-      <c r="I44" s="33"/>
+      <c r="I44" s="26"/>
     </row>
     <row r="45" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="17">
         <v>29</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="H45" s="39">
+      <c r="C45" s="23"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="29">
         <v>3</v>
       </c>
-      <c r="I45" s="33"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="17">
         <v>30</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" s="37"/>
-      <c r="F46" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="G46" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H46" s="39">
+      <c r="C46" s="23"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46" s="29">
         <v>3</v>
       </c>
-      <c r="I46" s="33"/>
+      <c r="I46" s="26"/>
     </row>
     <row r="47" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
-      <c r="C47" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="G47" s="60"/>
-      <c r="H47" s="39">
+      <c r="C47" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="80"/>
+      <c r="H47" s="29">
         <v>6</v>
       </c>
-      <c r="I47" s="33"/>
+      <c r="I47" s="26"/>
     </row>
     <row r="48" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="17">
         <v>31</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="H48" s="39">
+      <c r="C48" s="23"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="29">
         <v>2</v>
       </c>
-      <c r="I48" s="33"/>
+      <c r="I48" s="26"/>
     </row>
     <row r="49" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="17">
         <v>32</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37" t="s">
+      <c r="C49" s="23"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="H49" s="29">
+        <v>2</v>
+      </c>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="30">
+        <v>33</v>
+      </c>
+      <c r="C50" s="23"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="29">
+        <v>2</v>
+      </c>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="30"/>
+      <c r="C51" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="77"/>
+      <c r="H51" s="29">
+        <v>5</v>
+      </c>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="30">
+        <v>34</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="29">
+        <v>5</v>
+      </c>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="30"/>
+      <c r="C53" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="27"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" s="56"/>
+      <c r="H53" s="29">
+        <v>7</v>
+      </c>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="30">
+        <v>35</v>
+      </c>
+      <c r="C54" s="23"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="29">
+        <v>2</v>
+      </c>
+      <c r="I54" s="26"/>
+    </row>
+    <row r="55" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="30">
+        <v>36</v>
+      </c>
+      <c r="C55" s="23"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="H55" s="29">
+        <v>5</v>
+      </c>
+      <c r="I55" s="26"/>
+    </row>
+    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="30"/>
+      <c r="C56" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="27"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="G56" s="83"/>
+      <c r="H56" s="29">
+        <v>10</v>
+      </c>
+      <c r="I56" s="26"/>
+    </row>
+    <row r="57" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="30">
+        <v>37</v>
+      </c>
+      <c r="C57" s="23"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="H57" s="29">
+        <v>5</v>
+      </c>
+      <c r="I57" s="26"/>
+    </row>
+    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="30">
+        <v>38</v>
+      </c>
+      <c r="C58" s="23"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="G58" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="29">
+        <v>5</v>
+      </c>
+      <c r="I58" s="26"/>
+    </row>
+    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="30"/>
+      <c r="C59" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="27"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="G59" s="49"/>
+      <c r="H59" s="29">
+        <v>4</v>
+      </c>
+      <c r="I59" s="26"/>
+    </row>
+    <row r="60" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="30">
+        <v>39</v>
+      </c>
+      <c r="C60" s="23"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="G60" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" s="29">
+        <v>2</v>
+      </c>
+      <c r="I60" s="26"/>
+    </row>
+    <row r="61" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="30">
+        <v>40</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="29">
+        <v>2</v>
+      </c>
+      <c r="I61" s="26"/>
+    </row>
+    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="30"/>
+      <c r="C62" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="27"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="G62" s="77"/>
+      <c r="H62" s="29">
+        <v>5</v>
+      </c>
+      <c r="I62" s="26"/>
+    </row>
+    <row r="63" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="30">
+        <v>41</v>
+      </c>
+      <c r="C63" s="23"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="G63" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" s="29">
+        <v>5</v>
+      </c>
+      <c r="I63" s="26"/>
+    </row>
+    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="30"/>
+      <c r="C64" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="G64" s="77"/>
+      <c r="H64" s="29">
+        <v>8</v>
+      </c>
+      <c r="I64" s="26"/>
+    </row>
+    <row r="65" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="30">
+        <v>42</v>
+      </c>
+      <c r="C65" s="23"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F49" s="38" t="s">
+      <c r="H65" s="29">
+        <v>3</v>
+      </c>
+      <c r="I65" s="26"/>
+    </row>
+    <row r="66" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="30">
+        <v>43</v>
+      </c>
+      <c r="C66" s="23"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="79" t="s">
+        <v>91</v>
+      </c>
+      <c r="G66" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="H66" s="29">
+        <v>2</v>
+      </c>
+      <c r="I66" s="26"/>
+    </row>
+    <row r="67" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="30">
+        <v>44</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="G49" s="32" t="s">
+      <c r="G67" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="H49" s="39">
-        <v>2</v>
-      </c>
-      <c r="I49" s="33"/>
-    </row>
-    <row r="50" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="40">
-        <v>33</v>
-      </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F50" s="41" t="s">
+      <c r="H67" s="29">
+        <v>3</v>
+      </c>
+      <c r="I67" s="26"/>
+    </row>
+    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="30"/>
+      <c r="C68" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="27"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="G50" s="32" t="s">
+      <c r="G68" s="83"/>
+      <c r="H68" s="29">
+        <v>3</v>
+      </c>
+      <c r="I68" s="26"/>
+    </row>
+    <row r="69" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="30">
+        <v>45</v>
+      </c>
+      <c r="C69" s="23"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="H50" s="39">
-        <v>2</v>
-      </c>
-      <c r="I50" s="33"/>
-    </row>
-    <row r="51" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="40"/>
-      <c r="C51" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="59" t="s">
+      <c r="G69" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="59"/>
-      <c r="H51" s="39">
+      <c r="H69" s="29">
+        <v>3</v>
+      </c>
+      <c r="I69" s="26"/>
+    </row>
+    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="30"/>
+      <c r="C70" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D70" s="27"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70" s="83"/>
+      <c r="H70" s="29">
+        <v>6</v>
+      </c>
+      <c r="I70" s="26"/>
+    </row>
+    <row r="71" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="30">
+        <v>46</v>
+      </c>
+      <c r="C71" s="23"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="G71" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H71" s="29">
+        <v>3</v>
+      </c>
+      <c r="I71" s="26"/>
+    </row>
+    <row r="72" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="30">
+        <v>47</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="G72" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="29">
+        <v>3</v>
+      </c>
+      <c r="I72" s="26"/>
+    </row>
+    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="30"/>
+      <c r="C73" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D73" s="27"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="G73" s="83"/>
+      <c r="H73" s="29">
+        <v>11</v>
+      </c>
+      <c r="I73" s="26"/>
+    </row>
+    <row r="74" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="30">
+        <v>48</v>
+      </c>
+      <c r="C74" s="23"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="G74" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="H74" s="29">
+        <v>8</v>
+      </c>
+      <c r="I74" s="26"/>
+    </row>
+    <row r="75" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="31">
+        <v>49</v>
+      </c>
+      <c r="C75" s="32"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="85" t="s">
+        <v>106</v>
+      </c>
+      <c r="G75" s="85" t="s">
+        <v>107</v>
+      </c>
+      <c r="H75" s="35">
         <v>5</v>
       </c>
-      <c r="I51" s="33"/>
-    </row>
-    <row r="52" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="40">
-        <v>34</v>
-      </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="H52" s="39">
-        <v>5</v>
-      </c>
-      <c r="I52" s="33"/>
-    </row>
-    <row r="53" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="40"/>
-      <c r="C53" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="36"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="G53" s="59"/>
-      <c r="H53" s="39">
-        <v>7</v>
-      </c>
-      <c r="I53" s="33"/>
-    </row>
-    <row r="54" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="40">
-        <v>35</v>
-      </c>
-      <c r="C54" s="28"/>
-      <c r="D54" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="G54" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" s="39">
-        <v>2</v>
-      </c>
-      <c r="I54" s="33"/>
-    </row>
-    <row r="55" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="40">
-        <v>36</v>
-      </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="H55" s="39">
-        <v>5</v>
-      </c>
-      <c r="I55" s="33"/>
-    </row>
-    <row r="56" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="40"/>
-      <c r="C56" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="36"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="G56" s="59"/>
-      <c r="H56" s="39">
-        <v>10</v>
-      </c>
-      <c r="I56" s="33"/>
-    </row>
-    <row r="57" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="40">
-        <v>37</v>
-      </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="G57" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="H57" s="39">
-        <v>5</v>
-      </c>
-      <c r="I57" s="33"/>
-    </row>
-    <row r="58" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="40">
-        <v>38</v>
-      </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="G58" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="H58" s="39">
-        <v>5</v>
-      </c>
-      <c r="I58" s="33"/>
-    </row>
-    <row r="59" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="40"/>
-      <c r="C59" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" s="36"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="61"/>
-      <c r="H59" s="39">
-        <v>4</v>
-      </c>
-      <c r="I59" s="33"/>
-    </row>
-    <row r="60" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="40">
-        <v>39</v>
-      </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E60" s="37"/>
-      <c r="F60" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="G60" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="H60" s="39">
-        <v>2</v>
-      </c>
-      <c r="I60" s="33"/>
-    </row>
-    <row r="61" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="40">
-        <v>40</v>
-      </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="37"/>
-      <c r="F61" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="G61" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="H61" s="39">
-        <v>2</v>
-      </c>
-      <c r="I61" s="33"/>
-    </row>
-    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="40"/>
-      <c r="C62" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D62" s="36"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="G62" s="59"/>
-      <c r="H62" s="39">
-        <v>5</v>
-      </c>
-      <c r="I62" s="33"/>
-    </row>
-    <row r="63" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="40">
-        <v>41</v>
-      </c>
-      <c r="C63" s="28"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="G63" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="H63" s="39">
-        <v>5</v>
-      </c>
-      <c r="I63" s="33"/>
-    </row>
-    <row r="64" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="40"/>
-      <c r="C64" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="G64" s="59"/>
-      <c r="H64" s="39">
-        <v>8</v>
-      </c>
-      <c r="I64" s="33"/>
-    </row>
-    <row r="65" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="40">
-        <v>42</v>
-      </c>
-      <c r="C65" s="28"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H65" s="39">
-        <v>3</v>
-      </c>
-      <c r="I65" s="33"/>
-    </row>
-    <row r="66" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="40">
-        <v>43</v>
-      </c>
-      <c r="C66" s="28"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G66" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="H66" s="39">
-        <v>2</v>
-      </c>
-      <c r="I66" s="33"/>
-    </row>
-    <row r="67" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="40">
-        <v>44</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="G67" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="H67" s="39">
-        <v>3</v>
-      </c>
-      <c r="I67" s="33"/>
-    </row>
-    <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="40"/>
-      <c r="C68" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="D68" s="36"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="G68" s="59"/>
-      <c r="H68" s="39">
-        <v>3</v>
-      </c>
-      <c r="I68" s="33"/>
-    </row>
-    <row r="69" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="40">
-        <v>45</v>
-      </c>
-      <c r="C69" s="28"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="H69" s="39">
-        <v>3</v>
-      </c>
-      <c r="I69" s="33"/>
-    </row>
-    <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="40"/>
-      <c r="C70" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D70" s="36"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="G70" s="59"/>
-      <c r="H70" s="39">
-        <v>6</v>
-      </c>
-      <c r="I70" s="33"/>
-    </row>
-    <row r="71" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="40">
-        <v>46</v>
-      </c>
-      <c r="C71" s="28"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="G71" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="H71" s="39">
-        <v>3</v>
-      </c>
-      <c r="I71" s="33"/>
-    </row>
-    <row r="72" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="40">
-        <v>47</v>
-      </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="G72" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H72" s="39">
-        <v>3</v>
-      </c>
-      <c r="I72" s="33"/>
-    </row>
-    <row r="73" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="40"/>
-      <c r="C73" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D73" s="36"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="G73" s="59"/>
-      <c r="H73" s="39">
-        <v>11</v>
-      </c>
-      <c r="I73" s="33"/>
-    </row>
-    <row r="74" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="40">
-        <v>48</v>
-      </c>
-      <c r="C74" s="28"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="G74" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="H74" s="39">
-        <v>8</v>
-      </c>
-      <c r="I74" s="33"/>
-    </row>
-    <row r="75" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="44">
-        <v>49</v>
-      </c>
-      <c r="C75" s="45"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="G75" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="H75" s="49">
-        <v>5</v>
-      </c>
-      <c r="I75" s="50"/>
+      <c r="I75" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F56:G56"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="F64:G64"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E20">
@@ -3794,9 +3992,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>